<commit_message>
added transmission expansion to technology term
</commit_message>
<xml_diff>
--- a/data/pypsa_curtailment_emulator.xlsx
+++ b/data/pypsa_curtailment_emulator.xlsx
@@ -1816,22 +1816,22 @@
         <v>0</v>
       </c>
       <c r="E42" s="13" t="n">
-        <v>-0.03807920850308791</v>
+        <v>0.03807920850308791</v>
       </c>
       <c r="F42" s="13" t="n">
-        <v>-0.04926759243704416</v>
+        <v>0.04926759243704416</v>
       </c>
       <c r="G42" s="13" t="n">
-        <v>-0.1749825512014097</v>
+        <v>0.1749825512014097</v>
       </c>
       <c r="H42" s="13" t="n">
-        <v>-0.4657837775029747</v>
+        <v>0.4657837775029747</v>
       </c>
       <c r="I42" s="13" t="n">
-        <v>-0.3822968326306992</v>
+        <v>0.3822968326306992</v>
       </c>
       <c r="J42" s="13" t="n">
-        <v>-0.581644751777096</v>
+        <v>0.581644751777096</v>
       </c>
       <c r="L42" s="5" t="n"/>
       <c r="M42" s="5" t="n"/>
@@ -1845,25 +1845,25 @@
     <row r="43">
       <c r="C43" s="14" t="n"/>
       <c r="D43" s="2" t="n">
-        <v>-0.01419223246491806</v>
+        <v>0.01419223246491806</v>
       </c>
       <c r="E43" s="13" t="n">
-        <v>-0.1410778478247</v>
+        <v>0.1410778478247</v>
       </c>
       <c r="F43" s="13" t="n">
-        <v>-0.2251472196146845</v>
+        <v>0.2251472196146845</v>
       </c>
       <c r="G43" s="13" t="n">
-        <v>-0.3313660281446567</v>
+        <v>0.3313660281446567</v>
       </c>
       <c r="H43" s="13" t="n">
-        <v>-0.4351045304287916</v>
+        <v>0.4351045304287916</v>
       </c>
       <c r="I43" s="13" t="n">
-        <v>-0.5050387678763628</v>
+        <v>0.5050387678763628</v>
       </c>
       <c r="J43" s="13" t="n">
-        <v>-0.5553449424733008</v>
+        <v>0.5553449424733008</v>
       </c>
       <c r="L43" s="5" t="n"/>
       <c r="M43" s="5" t="n"/>
@@ -1877,25 +1877,25 @@
     <row r="44">
       <c r="C44" s="14" t="n"/>
       <c r="D44" s="2" t="n">
-        <v>-0.01624199507771802</v>
+        <v>0.01624199507771802</v>
       </c>
       <c r="E44" s="13" t="n">
-        <v>-0.1243593841431062</v>
+        <v>0.1243593841431062</v>
       </c>
       <c r="F44" s="13" t="n">
-        <v>-0.1782162170375382</v>
+        <v>0.1782162170375382</v>
       </c>
       <c r="G44" s="13" t="n">
-        <v>-0.228181530141783</v>
+        <v>0.228181530141783</v>
       </c>
       <c r="H44" s="13" t="n">
-        <v>-0.2765849466592284</v>
+        <v>0.2765849466592284</v>
       </c>
       <c r="I44" s="13" t="n">
-        <v>-0.3144327993924718</v>
+        <v>0.3144327993924718</v>
       </c>
       <c r="J44" s="13" t="n">
-        <v>-0.3003866169489345</v>
+        <v>0.3003866169489345</v>
       </c>
       <c r="L44" s="5" t="n"/>
       <c r="M44" s="5" t="n"/>
@@ -1910,22 +1910,22 @@
       <c r="B45" s="8" t="n"/>
       <c r="C45" s="14" t="n"/>
       <c r="D45" s="2" t="n">
-        <v>-0.01743064528986662</v>
+        <v>0.01743064528986662</v>
       </c>
       <c r="E45" s="13" t="n">
-        <v>-0.0898449861760492</v>
+        <v>0.0898449861760492</v>
       </c>
       <c r="F45" s="13" t="n">
-        <v>-0.106429764677167</v>
+        <v>0.106429764677167</v>
       </c>
       <c r="G45" s="13" t="n">
-        <v>-0.1190856003175532</v>
+        <v>0.1190856003175532</v>
       </c>
       <c r="H45" s="13" t="n">
-        <v>-0.1143818786250513</v>
+        <v>0.1143818786250513</v>
       </c>
       <c r="I45" s="13" t="n">
-        <v>-0.1430240986471133</v>
+        <v>0.1430240986471133</v>
       </c>
       <c r="J45" s="13" t="n">
         <v/>
@@ -1942,22 +1942,22 @@
     <row r="46">
       <c r="C46" s="14" t="n"/>
       <c r="D46" s="2" t="n">
-        <v>-0.01107935198956332</v>
+        <v>0.01107935198956332</v>
       </c>
       <c r="E46" s="13" t="n">
-        <v>-0.05180637406524109</v>
+        <v>0.05180637406524109</v>
       </c>
       <c r="F46" s="13" t="n">
-        <v>-0.04515241954845074</v>
+        <v>0.04515241954845074</v>
       </c>
       <c r="G46" s="13" t="n">
-        <v>-0.03699594123370264</v>
+        <v>0.03699594123370264</v>
       </c>
       <c r="H46" s="13" t="n">
-        <v>-0.007988524135573341</v>
+        <v>0.007988524135573341</v>
       </c>
       <c r="I46" s="13" t="n">
-        <v>-0.01591847493247362</v>
+        <v>0.01591847493247362</v>
       </c>
       <c r="J46" s="13" t="n">
         <v/>
@@ -1974,19 +1974,19 @@
     <row r="47">
       <c r="C47" s="14" t="n"/>
       <c r="D47" s="2" t="n">
-        <v>-0.005953797437680362</v>
+        <v>0.005953797437680362</v>
       </c>
       <c r="E47" s="13" t="n">
-        <v>-0.01871502997681276</v>
+        <v>0.01871502997681276</v>
       </c>
       <c r="F47" s="13" t="n">
-        <v>-0.004549167439444669</v>
+        <v>0.004549167439444669</v>
       </c>
       <c r="G47" s="13" t="n">
-        <v>0.03014924825547636</v>
+        <v>-0.03014924825547636</v>
       </c>
       <c r="H47" s="13" t="n">
-        <v>0.06856167593237956</v>
+        <v>-0.06856167593237956</v>
       </c>
       <c r="I47" s="13" t="n">
         <v/>
@@ -2006,13 +2006,13 @@
     <row r="48">
       <c r="C48" s="14" t="n"/>
       <c r="D48" s="2" t="n">
-        <v>-0.001004438729904129</v>
+        <v>0.001004438729904129</v>
       </c>
       <c r="E48" s="13" t="n">
-        <v>0.02035137001495592</v>
+        <v>-0.02035137001495592</v>
       </c>
       <c r="F48" s="13" t="n">
-        <v>0.05788503803984875</v>
+        <v>-0.05788503803984875</v>
       </c>
       <c r="G48" s="13" t="n">
         <v/>
@@ -2074,22 +2074,22 @@
         <v>0</v>
       </c>
       <c r="E51" s="13" t="n">
-        <v>-0.1510731638907951</v>
+        <v>0.1510731638907951</v>
       </c>
       <c r="F51" s="13" t="n">
-        <v>-0.2686526591317246</v>
+        <v>0.2686526591317246</v>
       </c>
       <c r="G51" s="13" t="n">
-        <v>-0.5130150794351762</v>
+        <v>0.5130150794351762</v>
       </c>
       <c r="H51" s="13" t="n">
-        <v>-0.6599230583560466</v>
+        <v>0.6599230583560466</v>
       </c>
       <c r="I51" s="13" t="n">
-        <v>-0.7761945502660924</v>
+        <v>0.7761945502660924</v>
       </c>
       <c r="J51" s="13" t="n">
-        <v>-1.084637948158285</v>
+        <v>1.084637948158285</v>
       </c>
       <c r="L51" s="5" t="n"/>
       <c r="M51" s="5" t="n"/>
@@ -2104,25 +2104,25 @@
     <row r="52">
       <c r="C52" s="14" t="n"/>
       <c r="D52" s="2" t="n">
-        <v>-0.001707913159101493</v>
+        <v>0.001707913159101493</v>
       </c>
       <c r="E52" s="13" t="n">
-        <v>-0.2539799277840126</v>
+        <v>0.2539799277840126</v>
       </c>
       <c r="F52" s="13" t="n">
-        <v>-0.6461515859087472</v>
+        <v>0.6461515859087472</v>
       </c>
       <c r="G52" s="13" t="n">
-        <v>-0.8739608739055509</v>
+        <v>0.8739608739055509</v>
       </c>
       <c r="H52" s="13" t="n">
-        <v>-1.121633891275849</v>
+        <v>1.121633891275849</v>
       </c>
       <c r="I52" s="13" t="n">
-        <v>-1.289035448916887</v>
+        <v>1.289035448916887</v>
       </c>
       <c r="J52" s="13" t="n">
-        <v>-1.444521156155731</v>
+        <v>1.444521156155731</v>
       </c>
       <c r="L52" s="5" t="n"/>
       <c r="M52" s="5" t="n"/>
@@ -2138,25 +2138,25 @@
     <row r="53">
       <c r="C53" s="14" t="n"/>
       <c r="D53" s="2" t="n">
-        <v>-0.004746608915359804</v>
+        <v>0.004746608915359804</v>
       </c>
       <c r="E53" s="13" t="n">
-        <v>-0.2683431549302445</v>
+        <v>0.2683431549302445</v>
       </c>
       <c r="F53" s="13" t="n">
-        <v>-0.5511170877225552</v>
+        <v>0.5511170877225552</v>
       </c>
       <c r="G53" s="13" t="n">
-        <v>-0.8510947657467732</v>
+        <v>0.8510947657467732</v>
       </c>
       <c r="H53" s="13" t="n">
-        <v>-1.077936295793381</v>
+        <v>1.077936295793381</v>
       </c>
       <c r="I53" s="13" t="n">
-        <v>-1.289670401863402</v>
+        <v>1.289670401863402</v>
       </c>
       <c r="J53" s="13" t="n">
-        <v>-1.119346987099373</v>
+        <v>1.119346987099373</v>
       </c>
       <c r="L53" s="5" t="n"/>
       <c r="M53" s="5" t="n"/>
@@ -2170,22 +2170,22 @@
     <row r="54">
       <c r="C54" s="14" t="n"/>
       <c r="D54" s="2" t="n">
-        <v>-0.04115880605720874</v>
+        <v>0.04115880605720874</v>
       </c>
       <c r="E54" s="13" t="n">
-        <v>-0.2097646454874569</v>
+        <v>0.2097646454874569</v>
       </c>
       <c r="F54" s="13" t="n">
-        <v>-0.5006630936993596</v>
+        <v>0.5006630936993596</v>
       </c>
       <c r="G54" s="13" t="n">
-        <v>-0.8274623592207895</v>
+        <v>0.8274623592207895</v>
       </c>
       <c r="H54" s="13" t="n">
-        <v>-1.061814793797657</v>
+        <v>1.061814793797657</v>
       </c>
       <c r="I54" s="13" t="n">
-        <v>-1.240909828752011</v>
+        <v>1.240909828752011</v>
       </c>
       <c r="J54" s="13" t="n">
         <v/>
@@ -2195,22 +2195,22 @@
       <c r="B55" s="8" t="n"/>
       <c r="C55" s="14" t="n"/>
       <c r="D55" s="2" t="n">
-        <v>-0.008558362859703005</v>
+        <v>0.008558362859703005</v>
       </c>
       <c r="E55" s="13" t="n">
-        <v>-0.1880232783644833</v>
+        <v>0.1880232783644833</v>
       </c>
       <c r="F55" s="13" t="n">
-        <v>-0.5170951321489407</v>
+        <v>0.5170951321489407</v>
       </c>
       <c r="G55" s="13" t="n">
-        <v>-0.7605002217647031</v>
+        <v>0.7605002217647031</v>
       </c>
       <c r="H55" s="13" t="n">
-        <v>-1.068166512772024</v>
+        <v>1.068166512772024</v>
       </c>
       <c r="I55" s="13" t="n">
-        <v>-1.094311838397483</v>
+        <v>1.094311838397483</v>
       </c>
       <c r="J55" s="13" t="n">
         <v/>
@@ -2221,19 +2221,19 @@
     <row r="56">
       <c r="C56" s="14" t="n"/>
       <c r="D56" s="2" t="n">
-        <v>-0.01243107319904072</v>
+        <v>0.01243107319904072</v>
       </c>
       <c r="E56" s="13" t="n">
-        <v>-0.2523794122609848</v>
+        <v>0.2523794122609848</v>
       </c>
       <c r="F56" s="13" t="n">
-        <v>-0.4962889934261825</v>
+        <v>0.4962889934261825</v>
       </c>
       <c r="G56" s="13" t="n">
-        <v>-0.7651035169817634</v>
+        <v>0.7651035169817634</v>
       </c>
       <c r="H56" s="13" t="n">
-        <v>-1.057533487248302</v>
+        <v>1.057533487248302</v>
       </c>
       <c r="I56" s="13" t="n">
         <v/>
@@ -2247,13 +2247,13 @@
     <row r="57">
       <c r="C57" s="14" t="n"/>
       <c r="D57" s="2" t="n">
-        <v>0.009400868951178839</v>
+        <v>-0.009400868951178839</v>
       </c>
       <c r="E57" s="13" t="n">
-        <v>-0.2687730762096723</v>
+        <v>0.2687730762096723</v>
       </c>
       <c r="F57" s="13" t="n">
-        <v>-0.5075483500591331</v>
+        <v>0.5075483500591331</v>
       </c>
       <c r="G57" s="13" t="n">
         <v/>
@@ -3644,22 +3644,22 @@
         <v>0</v>
       </c>
       <c r="E42" s="13" t="n">
-        <v>-0.0443934115864938</v>
+        <v>0.0443934115864938</v>
       </c>
       <c r="F42" s="13" t="n">
-        <v>-0.001336947024145993</v>
+        <v>0.001336947024145993</v>
       </c>
       <c r="G42" s="13" t="n">
-        <v>-0.03779790995251268</v>
+        <v>0.03779790995251268</v>
       </c>
       <c r="H42" s="13" t="n">
-        <v>-0.2192311907808228</v>
+        <v>0.2192311907808228</v>
       </c>
       <c r="I42" s="13" t="n">
-        <v>-0.2142824060512421</v>
+        <v>0.2142824060512421</v>
       </c>
       <c r="J42" s="13" t="n">
-        <v>-0.3109339512502715</v>
+        <v>0.3109339512502715</v>
       </c>
       <c r="L42" s="16" t="n"/>
       <c r="M42" s="16" t="n"/>
@@ -3673,25 +3673,25 @@
     <row r="43" ht="14.5" customHeight="1">
       <c r="C43" s="14" t="n"/>
       <c r="D43" s="2" t="n">
-        <v>7.170673537677454e-06</v>
+        <v>-7.170673537677454e-06</v>
       </c>
       <c r="E43" s="13" t="n">
-        <v>-0.04072135331409409</v>
+        <v>0.04072135331409409</v>
       </c>
       <c r="F43" s="13" t="n">
-        <v>-0.07424914552703732</v>
+        <v>0.07424914552703732</v>
       </c>
       <c r="G43" s="13" t="n">
-        <v>-0.06654355573083219</v>
+        <v>0.06654355573083219</v>
       </c>
       <c r="H43" s="13" t="n">
-        <v>-0.1122825620799758</v>
+        <v>0.1122825620799758</v>
       </c>
       <c r="I43" s="13" t="n">
-        <v>-0.1896266843091846</v>
+        <v>0.1896266843091846</v>
       </c>
       <c r="J43" s="13" t="n">
-        <v>-0.3501382794911784</v>
+        <v>0.3501382794911784</v>
       </c>
       <c r="L43" s="16" t="n"/>
       <c r="M43" s="16" t="n"/>
@@ -3705,25 +3705,25 @@
     <row r="44" ht="14.5" customHeight="1">
       <c r="C44" s="14" t="n"/>
       <c r="D44" s="2" t="n">
-        <v>-4.017680576350262e-05</v>
+        <v>4.017680576350262e-05</v>
       </c>
       <c r="E44" s="13" t="n">
-        <v>-0.02635004268088499</v>
+        <v>0.02635004268088499</v>
       </c>
       <c r="F44" s="13" t="n">
-        <v>-0.08416579132352937</v>
+        <v>0.08416579132352937</v>
       </c>
       <c r="G44" s="13" t="n">
-        <v>-0.1311721569005507</v>
+        <v>0.1311721569005507</v>
       </c>
       <c r="H44" s="13" t="n">
-        <v>-0.1290375611687204</v>
+        <v>0.1290375611687204</v>
       </c>
       <c r="I44" s="13" t="n">
-        <v>-0.1389185734277663</v>
+        <v>0.1389185734277663</v>
       </c>
       <c r="J44" s="13" t="n">
-        <v>-0.2176971956367648</v>
+        <v>0.2176971956367648</v>
       </c>
       <c r="L44" s="16" t="n"/>
       <c r="M44" s="16" t="n"/>
@@ -3737,22 +3737,22 @@
     <row r="45" ht="14.5" customHeight="1">
       <c r="C45" s="14" t="n"/>
       <c r="D45" s="2" t="n">
-        <v>-7.3482761622889e-05</v>
+        <v>7.3482761622889e-05</v>
       </c>
       <c r="E45" s="13" t="n">
-        <v>-0.0486254041774131</v>
+        <v>0.0486254041774131</v>
       </c>
       <c r="F45" s="13" t="n">
-        <v>-0.09222245664265515</v>
+        <v>0.09222245664265515</v>
       </c>
       <c r="G45" s="13" t="n">
-        <v>-0.1107917325037082</v>
+        <v>0.1107917325037082</v>
       </c>
       <c r="H45" s="13" t="n">
-        <v>-0.1403886811658372</v>
+        <v>0.1403886811658372</v>
       </c>
       <c r="I45" s="13" t="n">
-        <v>-0.07961127639709582</v>
+        <v>0.07961127639709582</v>
       </c>
       <c r="J45" s="13" t="n">
         <v/>
@@ -3769,22 +3769,22 @@
     <row r="46" ht="14.5" customHeight="1">
       <c r="C46" s="14" t="n"/>
       <c r="D46" s="2" t="n">
-        <v>-0.0001800821543901399</v>
+        <v>0.0001800821543901399</v>
       </c>
       <c r="E46" s="13" t="n">
-        <v>-0.04700598487038497</v>
+        <v>0.04700598487038497</v>
       </c>
       <c r="F46" s="13" t="n">
-        <v>-0.1134377019231578</v>
+        <v>0.1134377019231578</v>
       </c>
       <c r="G46" s="13" t="n">
-        <v>-0.1213465856756812</v>
+        <v>0.1213465856756812</v>
       </c>
       <c r="H46" s="13" t="n">
-        <v>-0.05223099867876894</v>
+        <v>0.05223099867876894</v>
       </c>
       <c r="I46" s="13" t="n">
-        <v>0.2204365736448612</v>
+        <v>-0.2204365736448612</v>
       </c>
       <c r="J46" s="13" t="n">
         <v/>
@@ -3801,19 +3801,19 @@
     <row r="47" ht="19.75" customHeight="1">
       <c r="C47" s="14" t="n"/>
       <c r="D47" s="2" t="n">
-        <v>-5.221878187348652e-05</v>
+        <v>5.221878187348652e-05</v>
       </c>
       <c r="E47" s="13" t="n">
-        <v>-0.05311464896388466</v>
+        <v>0.05311464896388466</v>
       </c>
       <c r="F47" s="13" t="n">
-        <v>-0.07875486248291225</v>
+        <v>0.07875486248291225</v>
       </c>
       <c r="G47" s="13" t="n">
-        <v>0.002089449809821217</v>
+        <v>-0.002089449809821217</v>
       </c>
       <c r="H47" s="13" t="n">
-        <v>0.2262773911747978</v>
+        <v>-0.2262773911747978</v>
       </c>
       <c r="I47" s="13" t="n">
         <v/>
@@ -3833,13 +3833,13 @@
     <row r="48" ht="14.5" customHeight="1">
       <c r="C48" s="14" t="n"/>
       <c r="D48" s="2" t="n">
-        <v>-0.0001483887263475372</v>
+        <v>0.0001483887263475372</v>
       </c>
       <c r="E48" s="13" t="n">
-        <v>-0.03927707482323817</v>
+        <v>0.03927707482323817</v>
       </c>
       <c r="F48" s="13" t="n">
-        <v>0.06147543694844773</v>
+        <v>-0.06147543694844773</v>
       </c>
       <c r="G48" s="13" t="n">
         <v/>
@@ -3899,22 +3899,22 @@
         <v>0</v>
       </c>
       <c r="E51" s="13" t="n">
-        <v>-0.2908328138323258</v>
+        <v>0.2908328138323258</v>
       </c>
       <c r="F51" s="13" t="n">
-        <v>-0.5096988584552465</v>
+        <v>0.5096988584552465</v>
       </c>
       <c r="G51" s="13" t="n">
-        <v>-0.7191890220212594</v>
+        <v>0.7191890220212594</v>
       </c>
       <c r="H51" s="13" t="n">
-        <v>-0.8732452277949271</v>
+        <v>0.8732452277949271</v>
       </c>
       <c r="I51" s="13" t="n">
-        <v>-0.9566724135629523</v>
+        <v>0.9566724135629523</v>
       </c>
       <c r="J51" s="13" t="n">
-        <v>-1.032973940284662</v>
+        <v>1.032973940284662</v>
       </c>
       <c r="L51" s="16" t="n"/>
       <c r="M51" s="16" t="n"/>
@@ -3929,25 +3929,25 @@
     <row r="52" ht="15.5" customHeight="1">
       <c r="C52" s="14" t="n"/>
       <c r="D52" s="2" t="n">
-        <v>-0.0005140527130918539</v>
+        <v>0.0005140527130918539</v>
       </c>
       <c r="E52" s="13" t="n">
-        <v>-0.320053997515194</v>
+        <v>0.320053997515194</v>
       </c>
       <c r="F52" s="13" t="n">
-        <v>-0.5696852569605324</v>
+        <v>0.5696852569605324</v>
       </c>
       <c r="G52" s="13" t="n">
-        <v>-0.7515295361662166</v>
+        <v>0.7515295361662166</v>
       </c>
       <c r="H52" s="13" t="n">
-        <v>-0.8811848077588235</v>
+        <v>0.8811848077588235</v>
       </c>
       <c r="I52" s="13" t="n">
-        <v>-0.9694244255569329</v>
+        <v>0.9694244255569329</v>
       </c>
       <c r="J52" s="13" t="n">
-        <v>-1.061241830821753</v>
+        <v>1.061241830821753</v>
       </c>
       <c r="L52" s="16" t="n"/>
       <c r="M52" s="16" t="n"/>
@@ -3963,25 +3963,25 @@
     <row r="53" ht="15.5" customHeight="1">
       <c r="C53" s="14" t="n"/>
       <c r="D53" s="2" t="n">
-        <v>-0.0005987242167493896</v>
+        <v>0.0005987242167493896</v>
       </c>
       <c r="E53" s="13" t="n">
-        <v>-0.3099320992833279</v>
+        <v>0.3099320992833279</v>
       </c>
       <c r="F53" s="13" t="n">
-        <v>-0.5692310729836303</v>
+        <v>0.5692310729836303</v>
       </c>
       <c r="G53" s="13" t="n">
-        <v>-0.7675684915317852</v>
+        <v>0.7675684915317852</v>
       </c>
       <c r="H53" s="13" t="n">
-        <v>-0.9039136213075745</v>
+        <v>0.9039136213075745</v>
       </c>
       <c r="I53" s="13" t="n">
-        <v>-0.9952994996996426</v>
+        <v>0.9952994996996426</v>
       </c>
       <c r="J53" s="13" t="n">
-        <v>-1.100508264115412</v>
+        <v>1.100508264115412</v>
       </c>
       <c r="L53" s="16" t="n"/>
       <c r="M53" s="16" t="n"/>
@@ -3995,22 +3995,22 @@
     <row r="54">
       <c r="C54" s="14" t="n"/>
       <c r="D54" s="2" t="n">
-        <v>-0.001236127776125065</v>
+        <v>0.001236127776125065</v>
       </c>
       <c r="E54" s="13" t="n">
-        <v>-0.2991250808544557</v>
+        <v>0.2991250808544557</v>
       </c>
       <c r="F54" s="13" t="n">
-        <v>-0.573643424832342</v>
+        <v>0.573643424832342</v>
       </c>
       <c r="G54" s="13" t="n">
-        <v>-0.7838988623476733</v>
+        <v>0.7838988623476733</v>
       </c>
       <c r="H54" s="13" t="n">
-        <v>-0.9295001512731182</v>
+        <v>0.9295001512731182</v>
       </c>
       <c r="I54" s="13" t="n">
-        <v>-1.034899869980614</v>
+        <v>1.034899869980614</v>
       </c>
       <c r="J54" s="13" t="n">
         <v/>
@@ -4019,22 +4019,22 @@
     <row r="55">
       <c r="C55" s="14" t="n"/>
       <c r="D55" s="2" t="n">
-        <v>-0.001239739247778578</v>
+        <v>0.001239739247778578</v>
       </c>
       <c r="E55" s="13" t="n">
-        <v>-0.2911804032713267</v>
+        <v>0.2911804032713267</v>
       </c>
       <c r="F55" s="13" t="n">
-        <v>-0.5816092507080989</v>
+        <v>0.5816092507080989</v>
       </c>
       <c r="G55" s="13" t="n">
-        <v>-0.8071614649744907</v>
+        <v>0.8071614649744907</v>
       </c>
       <c r="H55" s="13" t="n">
-        <v>-0.9596811512954909</v>
+        <v>0.9596811512954909</v>
       </c>
       <c r="I55" s="13" t="n">
-        <v>-1.066464881058169</v>
+        <v>1.066464881058169</v>
       </c>
       <c r="J55" s="13" t="n">
         <v/>
@@ -4045,19 +4045,19 @@
     <row r="56">
       <c r="C56" s="14" t="n"/>
       <c r="D56" s="2" t="n">
-        <v>-0.002206986528664534</v>
+        <v>0.002206986528664534</v>
       </c>
       <c r="E56" s="13" t="n">
-        <v>-0.2773199247978722</v>
+        <v>0.2773199247978722</v>
       </c>
       <c r="F56" s="13" t="n">
-        <v>-0.5975804945647406</v>
+        <v>0.5975804945647406</v>
       </c>
       <c r="G56" s="13" t="n">
-        <v>-0.828242120952577</v>
+        <v>0.828242120952577</v>
       </c>
       <c r="H56" s="13" t="n">
-        <v>-0.9711025010416207</v>
+        <v>0.9711025010416207</v>
       </c>
       <c r="I56" s="13" t="n">
         <v/>
@@ -4071,13 +4071,13 @@
     <row r="57">
       <c r="C57" s="14" t="n"/>
       <c r="D57" s="2" t="n">
-        <v>-0.004687280317108817</v>
+        <v>0.004687280317108817</v>
       </c>
       <c r="E57" s="13" t="n">
-        <v>-0.2574871344819252</v>
+        <v>0.2574871344819252</v>
       </c>
       <c r="F57" s="13" t="n">
-        <v>-0.6079428170164718</v>
+        <v>0.6079428170164718</v>
       </c>
       <c r="G57" s="13" t="n">
         <v/>

</xml_diff>